<commit_message>
Updated Excel file via Streamlit app
</commit_message>
<xml_diff>
--- a/Vehicle_Checkout_List.xlsx
+++ b/Vehicle_Checkout_List.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bre Powers</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -530,10 +530,10 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45600</v>
+        <v>45567</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45600</v>
+        <v>45568</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
@@ -554,7 +554,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -563,19 +563,17 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45595</v>
+        <v>45421</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>45596</v>
+        <v>45421</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
         </is>
       </c>
-      <c r="G4" t="n">
-        <v>315</v>
-      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
         <v>17</v>
@@ -587,7 +585,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bre Powers</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -596,18 +594,20 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45593</v>
+        <v>45432</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>45593</v>
+        <v>45538</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
         </is>
       </c>
-      <c r="G5" t="n">
-        <v>313</v>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>California all summer</t>
+        </is>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
@@ -629,10 +629,10 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>45581</v>
+        <v>45546</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>45582</v>
+        <v>45547</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -662,10 +662,10 @@
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>45579</v>
+        <v>45551</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>45579</v>
+        <v>45551</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
@@ -695,20 +695,18 @@
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>45576</v>
+        <v>45553</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>45576</v>
+        <v>45554</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>field work near flagstaff</t>
-        </is>
+      <c r="G8" t="n">
+        <v>315</v>
       </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
@@ -721,7 +719,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>Bre Powers</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -730,10 +728,10 @@
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>45574</v>
+        <v>45558</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>45575</v>
+        <v>45558</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -741,7 +739,7 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
@@ -754,7 +752,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Bre Powers</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -763,10 +761,10 @@
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>45572</v>
+        <v>45560</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>45572</v>
+        <v>45561</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -774,7 +772,7 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
@@ -787,7 +785,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>Derek Uhey</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -796,19 +794,17 @@
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>45588</v>
+        <v>45539</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>45589</v>
+        <v>45540</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
         </is>
       </c>
-      <c r="G11" t="n">
-        <v>315</v>
-      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
         <v>15</v>
@@ -820,7 +816,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>Bre Powers</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -829,10 +825,10 @@
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>45560</v>
+        <v>45572</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>45561</v>
+        <v>45572</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -840,7 +836,7 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
@@ -853,7 +849,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Bre Powers</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -862,10 +858,10 @@
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>45558</v>
+        <v>45574</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>45558</v>
+        <v>45575</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -873,7 +869,7 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="n">
@@ -895,18 +891,20 @@
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>45553</v>
+        <v>45576</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>45554</v>
+        <v>45576</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
         </is>
       </c>
-      <c r="G14" t="n">
-        <v>315</v>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>field work near flagstaff</t>
+        </is>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="n">
@@ -928,10 +926,10 @@
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>45551</v>
+        <v>45579</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>45551</v>
+        <v>45579</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -939,7 +937,7 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
@@ -961,10 +959,10 @@
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>45546</v>
+        <v>45581</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>45547</v>
+        <v>45582</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -985,7 +983,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Derek Uhey</t>
+          <t>Bre Powers</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -994,17 +992,19 @@
         </is>
       </c>
       <c r="D17" s="2" t="n">
-        <v>45539</v>
+        <v>45593</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>45540</v>
+        <v>45593</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
           <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr"/>
+      <c r="G17" t="n">
+        <v>313</v>
+      </c>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="n">
         <v>3</v>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1025,20 +1025,18 @@
         </is>
       </c>
       <c r="D18" s="2" t="n">
-        <v>45432</v>
+        <v>45595</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>45538</v>
+        <v>45596</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
           <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>California all summer</t>
-        </is>
+      <c r="G18" t="n">
+        <v>315</v>
       </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="n">
@@ -1051,7 +1049,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>Bre Powers</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1060,17 +1058,19 @@
         </is>
       </c>
       <c r="D19" s="2" t="n">
-        <v>45421</v>
+        <v>45600</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>45421</v>
+        <v>45600</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
           <t>268 - 2017 Ford F-150, Silver(6 Seats)</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>313</v>
+      </c>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="n">
         <v>1</v>
@@ -1091,10 +1091,10 @@
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>45567</v>
+        <v>45588</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>45568</v>
+        <v>45589</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Ben</t>
+          <t>Max Yusen</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1124,17 +1124,21 @@
         </is>
       </c>
       <c r="D21" s="2" t="n">
-        <v>45637</v>
+        <v>45594</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>45642</v>
+        <v>45595</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
           <t>310 - Chevy Trail Boss, White</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>AZWI</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
         <v>26</v>
@@ -1146,7 +1150,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>keven</t>
+          <t>Adair Patterson</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1155,21 +1159,17 @@
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>45627</v>
+        <v>45554</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>45635</v>
+        <v>45556</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>310 - Chevy Trail Boss, White</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">We will be traveling to Organ Pipe, Casa Grande, and Tonto National monuments to conduct fieldwork for my PhD project. The vehicle will be used to transport people and materials for that work. We will have no more than 4 people in the vehicle. </t>
-        </is>
-      </c>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
         <v>25</v>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Andrew Henning</t>
+          <t>Max Yusen</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1190,10 +1190,10 @@
         </is>
       </c>
       <c r="D23" s="2" t="n">
-        <v>45605</v>
+        <v>45588</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>45610</v>
+        <v>45588</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1202,7 +1202,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Down to the valley for a conference </t>
+          <t>AZWI</t>
         </is>
       </c>
       <c r="H23" t="inlineStr"/>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Max Yusen</t>
+          <t>Darren Olney</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1225,10 +1225,10 @@
         </is>
       </c>
       <c r="D24" s="2" t="n">
-        <v>45600</v>
+        <v>45581</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>45600</v>
+        <v>45585</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>AZWI</t>
+          <t>POC: deo73@nau.edu</t>
         </is>
       </c>
       <c r="H24" t="inlineStr"/>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Darren Olney</t>
+          <t>keven</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1260,10 +1260,10 @@
         </is>
       </c>
       <c r="D25" s="2" t="n">
-        <v>45581</v>
+        <v>45627</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>45585</v>
+        <v>45635</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>POC: deo73@nau.edu</t>
+          <t xml:space="preserve">We will be traveling to Organ Pipe, Casa Grande, and Tonto National monuments to conduct fieldwork for my PhD project. The vehicle will be used to transport people and materials for that work. We will have no more than 4 people in the vehicle. </t>
         </is>
       </c>
       <c r="H25" t="inlineStr"/>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Max Yusen</t>
+          <t>Andrew Henning</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1295,10 +1295,10 @@
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>45588</v>
+        <v>45605</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>45588</v>
+        <v>45610</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>AZWI</t>
+          <t xml:space="preserve">Down to the valley for a conference </t>
         </is>
       </c>
       <c r="H26" t="inlineStr"/>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Adair Patterson</t>
+          <t>Ben</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1330,10 +1330,10 @@
         </is>
       </c>
       <c r="D27" s="2" t="n">
-        <v>45554</v>
+        <v>45637</v>
       </c>
       <c r="E27" s="2" t="n">
-        <v>45556</v>
+        <v>45642</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1361,10 +1361,10 @@
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>45594</v>
+        <v>45600</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>45595</v>
+        <v>45600</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>jaime</t>
+          <t>Margaret Moore</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1396,10 +1396,10 @@
         </is>
       </c>
       <c r="D29" s="2" t="n">
-        <v>45603</v>
+        <v>45581</v>
       </c>
       <c r="E29" s="2" t="n">
-        <v>45604</v>
+        <v>45587</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>SRP field work</t>
+          <t>SAEF</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
@@ -1431,26 +1431,18 @@
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>45627</v>
+        <v>45589</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>45748</v>
+        <v>45593</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
           <t>321 - Chevy Trail Boss, White</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">This vehicle will be used to travel to the Sierra Ancha Experimental Forest throughout the winter months to collect snow, snow melt, and stream samples for water stable isotopes and chemistry. </t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>Emory Ellis</t>
-        </is>
-      </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
       <c r="I30" t="n">
         <v>36</v>
       </c>
@@ -1461,7 +1453,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Max Yusen</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1470,21 +1462,17 @@
         </is>
       </c>
       <c r="D31" s="2" t="n">
-        <v>45611</v>
+        <v>45562</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>45611</v>
+        <v>45564</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
           <t>321 - Chevy Trail Boss, White</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>school to teach about fire for a day</t>
-        </is>
-      </c>
+      <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="n">
         <v>35</v>
@@ -1496,7 +1484,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Cat</t>
+          <t>David Auty</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1505,21 +1493,17 @@
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>45608</v>
+        <v>45568</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>45608</v>
+        <v>45568</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
           <t>321 - Chevy Trail Boss, White</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Payson for a workshop</t>
-        </is>
-      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="n">
         <v>34</v>
@@ -1531,7 +1515,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Megan Rangel-Lynch</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1540,10 +1524,10 @@
         </is>
       </c>
       <c r="D33" s="2" t="n">
-        <v>45597</v>
+        <v>45548</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>45598</v>
+        <v>45554</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1562,7 +1546,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>jaime</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1571,17 +1555,21 @@
         </is>
       </c>
       <c r="D34" s="2" t="n">
-        <v>45548</v>
+        <v>45603</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>45554</v>
+        <v>45604</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
           <t>321 - Chevy Trail Boss, White</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>SRP field work</t>
+        </is>
+      </c>
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="n">
         <v>27</v>
@@ -1593,7 +1581,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Margaret Moore</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1602,10 +1590,10 @@
         </is>
       </c>
       <c r="D35" s="2" t="n">
-        <v>45581</v>
+        <v>45608</v>
       </c>
       <c r="E35" s="2" t="n">
-        <v>45587</v>
+        <v>45608</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1614,7 +1602,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>SAEF</t>
+          <t>Payson for a workshop</t>
         </is>
       </c>
       <c r="H35" t="inlineStr"/>
@@ -1628,7 +1616,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>David Auty</t>
+          <t>Max Yusen</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1637,17 +1625,21 @@
         </is>
       </c>
       <c r="D36" s="2" t="n">
-        <v>45568</v>
+        <v>45611</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>45568</v>
+        <v>45611</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
           <t>321 - Chevy Trail Boss, White</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr"/>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>school to teach about fire for a day</t>
+        </is>
+      </c>
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="n">
         <v>29</v>
@@ -1659,7 +1651,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Emory Ellis</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1668,18 +1660,26 @@
         </is>
       </c>
       <c r="D37" s="2" t="n">
-        <v>45562</v>
+        <v>45627</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>45564</v>
+        <v>45748</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
           <t>321 - Chevy Trail Boss, White</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This vehicle will be used to travel to the Sierra Ancha Experimental Forest throughout the winter months to collect snow, snow melt, and stream samples for water stable isotopes and chemistry. </t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Emory Ellis</t>
+        </is>
+      </c>
       <c r="I37" t="n">
         <v>28</v>
       </c>
@@ -1690,7 +1690,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Emory Ellis</t>
+          <t>Megan Rangel-Lynch</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1699,10 +1699,10 @@
         </is>
       </c>
       <c r="D38" s="2" t="n">
-        <v>45589</v>
+        <v>45597</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>45593</v>
+        <v>45598</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1951,10 +1951,10 @@
         </is>
       </c>
       <c r="D46" s="2" t="n">
-        <v>45642</v>
+        <v>45581</v>
       </c>
       <c r="E46" s="2" t="n">
-        <v>45643</v>
+        <v>45583</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -1963,14 +1963,10 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Andrei will be joining us in the field (as long as he is feeling better) in Superior, AZ. The fieldwork is being conducted as part of my PhD research.</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>Keven Griffen</t>
-        </is>
-      </c>
+          <t>for keven, srp data collection</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr"/>
       <c r="I46" t="n">
         <v>49</v>
       </c>
@@ -1981,7 +1977,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1990,10 +1986,10 @@
         </is>
       </c>
       <c r="D47" s="2" t="n">
-        <v>45595</v>
+        <v>45576</v>
       </c>
       <c r="E47" s="2" t="n">
-        <v>45595</v>
+        <v>45576</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -2012,7 +2008,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2021,10 +2017,10 @@
         </is>
       </c>
       <c r="D48" s="2" t="n">
-        <v>45588</v>
+        <v>45565</v>
       </c>
       <c r="E48" s="2" t="n">
-        <v>45588</v>
+        <v>45567</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -2043,7 +2039,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Cat</t>
+          <t>Bowker</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2052,18 +2048,26 @@
         </is>
       </c>
       <c r="D49" s="2" t="n">
-        <v>45565</v>
+        <v>45642</v>
       </c>
       <c r="E49" s="2" t="n">
-        <v>45567</v>
+        <v>45643</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
           <t>329 - Chevy Trail Boss, White</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Andrei will be joining us in the field (as long as he is feeling better) in Superior, AZ. The fieldwork is being conducted as part of my PhD research.</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Keven Griffen</t>
+        </is>
+      </c>
       <c r="I49" t="n">
         <v>44</v>
       </c>
@@ -2074,7 +2078,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2083,10 +2087,10 @@
         </is>
       </c>
       <c r="D50" s="2" t="n">
-        <v>45576</v>
+        <v>45595</v>
       </c>
       <c r="E50" s="2" t="n">
-        <v>45576</v>
+        <v>45595</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2105,7 +2109,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Bowker</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2114,21 +2118,17 @@
         </is>
       </c>
       <c r="D51" s="2" t="n">
-        <v>45581</v>
+        <v>45588</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>45583</v>
+        <v>45588</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
           <t>329 - Chevy Trail Boss, White</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>for keven, srp data collection</t>
-        </is>
-      </c>
+      <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="n">
         <v>46</v>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Kimberly Walker</t>
+          <t>Wade Axup</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2184,18 +2184,26 @@
         </is>
       </c>
       <c r="D53" s="2" t="n">
-        <v>45611</v>
+        <v>45572</v>
       </c>
       <c r="E53" s="2" t="n">
-        <v>45611</v>
+        <v>45576</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
           <t>331- 2024  Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>This minivan is being requested to support staff/faculty travel to the AZ Tribal Fire &amp; Climate Resilience Summit, which is hosted by the AZWI and SWFSC.</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Wade Axup</t>
+        </is>
+      </c>
       <c r="I53" t="n">
         <v>57</v>
       </c>
@@ -2206,7 +2214,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Colin Whitehead</t>
+          <t>Michael Sloan</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2215,24 +2223,20 @@
         </is>
       </c>
       <c r="D54" s="2" t="n">
-        <v>45642</v>
+        <v>45481</v>
       </c>
       <c r="E54" s="2" t="n">
-        <v>45642</v>
+        <v>45490</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
           <t>331- 2024  Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Heading down to Prescott AZ for a third grade school visit; presenting fire ecology. </t>
-        </is>
-      </c>
+      <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>{Colin Whitehead}{Max yusen}{Cole Brant}</t>
+          <t>Jasmine Anenberg</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -2245,7 +2249,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Wade Axup</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2254,24 +2258,20 @@
         </is>
       </c>
       <c r="D55" s="2" t="n">
-        <v>45629</v>
+        <v>45503</v>
       </c>
       <c r="E55" s="2" t="n">
-        <v>45633</v>
+        <v>45503</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
           <t>331- 2024  Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t xml:space="preserve">	This minivan is being requested to support staff/faculty travel to the AZ Wildland Urban Interface Summit, which is being planned and hosted by the AZWI &amp; SWFSC.</t>
-        </is>
-      </c>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Wade Axup</t>
+          <t>Shay Levine</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -2284,7 +2284,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Wade Axup</t>
+          <t>Michael Sloan</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2293,10 +2293,10 @@
         </is>
       </c>
       <c r="D56" s="2" t="n">
-        <v>45613</v>
+        <v>45534</v>
       </c>
       <c r="E56" s="2" t="n">
-        <v>45619</v>
+        <v>45553</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -2305,25 +2305,21 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>This minivan is being requested to support staff/faculty travel to the Southwest Fire Ecology Conference, which is hosted and planned by the AZWI and SWFSC.</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>Wade Axup</t>
-        </is>
-      </c>
+          <t xml:space="preserve">transporting Dirt lab grad students and technicians to Jerome, AZ for a lab training event. </t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr"/>
       <c r="I56" t="n">
         <v>58</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Hofstetter</t>
+          <t>David Auty</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2332,21 +2328,17 @@
         </is>
       </c>
       <c r="D57" s="2" t="n">
-        <v>45605</v>
+        <v>45568</v>
       </c>
       <c r="E57" s="2" t="n">
-        <v>45609</v>
+        <v>45568</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
           <t>331- 2024  Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t xml:space="preserve">drive to Phoenix for a conference </t>
-        </is>
-      </c>
+      <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="n">
         <v>56</v>
@@ -2354,11 +2346,11 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>David Auty</t>
+          <t>Wade Axup</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2367,18 +2359,26 @@
         </is>
       </c>
       <c r="D58" s="2" t="n">
-        <v>45568</v>
+        <v>45613</v>
       </c>
       <c r="E58" s="2" t="n">
-        <v>45568</v>
+        <v>45619</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
           <t>331- 2024  Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="inlineStr"/>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>This minivan is being requested to support staff/faculty travel to the Southwest Fire Ecology Conference, which is hosted and planned by the AZWI and SWFSC.</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Wade Axup</t>
+        </is>
+      </c>
       <c r="I58" t="n">
         <v>54</v>
       </c>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Wade Axup</t>
+          <t>Hofstetter</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2398,10 +2398,10 @@
         </is>
       </c>
       <c r="D59" s="2" t="n">
-        <v>45572</v>
+        <v>45605</v>
       </c>
       <c r="E59" s="2" t="n">
-        <v>45576</v>
+        <v>45609</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
@@ -2410,14 +2410,10 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>This minivan is being requested to support staff/faculty travel to the AZ Tribal Fire &amp; Climate Resilience Summit, which is hosted by the AZWI and SWFSC.</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>Wade Axup</t>
-        </is>
-      </c>
+          <t xml:space="preserve">drive to Phoenix for a conference </t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr"/>
       <c r="I59" t="n">
         <v>55</v>
       </c>
@@ -2428,7 +2424,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Michael Sloan</t>
+          <t>Wade Axup</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2437,10 +2433,10 @@
         </is>
       </c>
       <c r="D60" s="2" t="n">
-        <v>45534</v>
+        <v>45629</v>
       </c>
       <c r="E60" s="2" t="n">
-        <v>45553</v>
+        <v>45633</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -2449,10 +2445,14 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t xml:space="preserve">transporting Dirt lab grad students and technicians to Jerome, AZ for a lab training event. </t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr"/>
+          <t xml:space="preserve">	This minivan is being requested to support staff/faculty travel to the AZ Wildland Urban Interface Summit, which is being planned and hosted by the AZWI &amp; SWFSC.</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Wade Axup</t>
+        </is>
+      </c>
       <c r="I60" t="n">
         <v>53</v>
       </c>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>Colin Whitehead</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2472,20 +2472,24 @@
         </is>
       </c>
       <c r="D61" s="2" t="n">
-        <v>45503</v>
+        <v>45642</v>
       </c>
       <c r="E61" s="2" t="n">
-        <v>45503</v>
+        <v>45642</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
           <t>331- 2024  Toyota Sienna Hybrid, White (8 seats)</t>
         </is>
       </c>
-      <c r="G61" t="inlineStr"/>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Heading down to Prescott AZ for a third grade school visit; presenting fire ecology. </t>
+        </is>
+      </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Shay Levine</t>
+          <t>{Colin Whitehead}{Max yusen}{Cole Brant}</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -2498,7 +2502,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Michael Sloan</t>
+          <t>Kimberly Walker</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2507,10 +2511,10 @@
         </is>
       </c>
       <c r="D62" s="2" t="n">
-        <v>45481</v>
+        <v>45611</v>
       </c>
       <c r="E62" s="2" t="n">
-        <v>45490</v>
+        <v>45611</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -2518,11 +2522,7 @@
         </is>
       </c>
       <c r="G62" t="inlineStr"/>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>Jasmine Anenberg</t>
-        </is>
-      </c>
+      <c r="H62" t="inlineStr"/>
       <c r="I62" t="n">
         <v>51</v>
       </c>
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Anita</t>
+          <t>Anita Joy Antoninka</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2826,17 +2826,21 @@
         </is>
       </c>
       <c r="D71" s="2" t="n">
-        <v>45627</v>
+        <v>45444</v>
       </c>
       <c r="E71" s="2" t="n">
-        <v>45636</v>
+        <v>45536</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="G71" t="inlineStr"/>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>New Mexico, dates not needed are TBD</t>
+        </is>
+      </c>
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="n">
         <v>77</v>
@@ -2848,7 +2852,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Anita</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2857,10 +2861,10 @@
         </is>
       </c>
       <c r="D72" s="2" t="n">
-        <v>45617</v>
+        <v>45421</v>
       </c>
       <c r="E72" s="2" t="n">
-        <v>45623</v>
+        <v>45421</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -2879,7 +2883,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Anita</t>
+          <t>Michael Sloan</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2888,10 +2892,10 @@
         </is>
       </c>
       <c r="D73" s="2" t="n">
-        <v>45602</v>
+        <v>45422</v>
       </c>
       <c r="E73" s="2" t="n">
-        <v>45608</v>
+        <v>45427</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
@@ -2910,7 +2914,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Michael Sloan</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2919,21 +2923,17 @@
         </is>
       </c>
       <c r="D74" s="2" t="n">
-        <v>45541</v>
+        <v>45432</v>
       </c>
       <c r="E74" s="2" t="n">
-        <v>45571</v>
+        <v>45433</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Truck will be used to drive 4 students and gear to Valles Caldera Preserve in New Mexico. It will transport the techs around the preserve on some bad roads to the 12 field sites we have in the area. </t>
-        </is>
-      </c>
+      <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="n">
         <v>74</v>
@@ -2945,7 +2945,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Anita</t>
+          <t>Olsen</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2954,10 +2954,10 @@
         </is>
       </c>
       <c r="D75" s="2" t="n">
-        <v>45639</v>
+        <v>45401</v>
       </c>
       <c r="E75" s="2" t="n">
-        <v>45647</v>
+        <v>45402</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
@@ -2976,7 +2976,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Michael Sloan</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2985,17 +2985,21 @@
         </is>
       </c>
       <c r="D76" s="2" t="n">
-        <v>45432</v>
+        <v>45541</v>
       </c>
       <c r="E76" s="2" t="n">
-        <v>45433</v>
+        <v>45571</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="G76" t="inlineStr"/>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Truck will be used to drive 4 students and gear to Valles Caldera Preserve in New Mexico. It will transport the techs around the preserve on some bad roads to the 12 field sites we have in the area. </t>
+        </is>
+      </c>
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="n">
         <v>72</v>
@@ -3007,7 +3011,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Michael Sloan</t>
+          <t>Anita</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3016,10 +3020,10 @@
         </is>
       </c>
       <c r="D77" s="2" t="n">
-        <v>45422</v>
+        <v>45602</v>
       </c>
       <c r="E77" s="2" t="n">
-        <v>45427</v>
+        <v>45608</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
@@ -3038,7 +3042,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>Anita</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3047,10 +3051,10 @@
         </is>
       </c>
       <c r="D78" s="2" t="n">
-        <v>45421</v>
+        <v>45617</v>
       </c>
       <c r="E78" s="2" t="n">
-        <v>45421</v>
+        <v>45623</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
@@ -3069,7 +3073,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Anita Joy Antoninka</t>
+          <t>Anita</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3078,21 +3082,17 @@
         </is>
       </c>
       <c r="D79" s="2" t="n">
-        <v>45444</v>
+        <v>45639</v>
       </c>
       <c r="E79" s="2" t="n">
-        <v>45536</v>
+        <v>45647</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
           <t>333 - 2017 Toyota Tacoma, Charcoal (5 Seats)</t>
         </is>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>New Mexico, dates not needed are TBD</t>
-        </is>
-      </c>
+      <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr"/>
       <c r="I79" t="n">
         <v>73</v>
@@ -3104,7 +3104,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Olsen</t>
+          <t>Anita</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3113,10 +3113,10 @@
         </is>
       </c>
       <c r="D80" s="2" t="n">
-        <v>45401</v>
+        <v>45627</v>
       </c>
       <c r="E80" s="2" t="n">
-        <v>45402</v>
+        <v>45636</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
@@ -3135,7 +3135,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Margaret Moore</t>
+          <t>Seafha Ramos</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3144,21 +3144,17 @@
         </is>
       </c>
       <c r="D81" s="2" t="n">
-        <v>45581</v>
+        <v>45403</v>
       </c>
       <c r="E81" s="2" t="n">
-        <v>45587</v>
+        <v>45423</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>SAEF</t>
-        </is>
-      </c>
+      <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
       <c r="I81" t="n">
         <v>83</v>
@@ -3170,7 +3166,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Seafha Ramos</t>
+          <t>Margaret Moore</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3179,10 +3175,10 @@
         </is>
       </c>
       <c r="D82" s="2" t="n">
-        <v>45597</v>
+        <v>45425</v>
       </c>
       <c r="E82" s="2" t="n">
-        <v>45613</v>
+        <v>45474</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
@@ -3191,7 +3187,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Day use in town for the extent of stay</t>
+          <t>Tonto/ dates not needed TBD</t>
         </is>
       </c>
       <c r="H82" t="inlineStr"/>
@@ -3205,7 +3201,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Cat</t>
+          <t>Bowker</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3214,21 +3210,17 @@
         </is>
       </c>
       <c r="D83" s="2" t="n">
-        <v>45594</v>
+        <v>45401</v>
       </c>
       <c r="E83" s="2" t="n">
-        <v>45594</v>
+        <v>45402</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t xml:space="preserve">FOR445 related field trip destination wilderness either in Sedona, Sycamore canyon, or around Flagstaff </t>
-        </is>
-      </c>
+      <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
       <c r="I83" t="n">
         <v>84</v>
@@ -3284,17 +3276,21 @@
         </is>
       </c>
       <c r="D85" s="2" t="n">
-        <v>45403</v>
+        <v>45597</v>
       </c>
       <c r="E85" s="2" t="n">
-        <v>45423</v>
+        <v>45613</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="G85" t="inlineStr"/>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Day use in town for the extent of stay</t>
+        </is>
+      </c>
       <c r="H85" t="inlineStr"/>
       <c r="I85" t="n">
         <v>80</v>
@@ -3306,7 +3302,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Bowker</t>
+          <t>Margaret Moore</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3315,17 +3311,21 @@
         </is>
       </c>
       <c r="D86" s="2" t="n">
-        <v>45401</v>
+        <v>45581</v>
       </c>
       <c r="E86" s="2" t="n">
-        <v>45402</v>
+        <v>45587</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
           <t>338 - 2012 Nissan Titan, White (5 Seats)</t>
         </is>
       </c>
-      <c r="G86" t="inlineStr"/>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>SAEF</t>
+        </is>
+      </c>
       <c r="H86" t="inlineStr"/>
       <c r="I86" t="n">
         <v>79</v>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Margaret Moore</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3346,10 +3346,10 @@
         </is>
       </c>
       <c r="D87" s="2" t="n">
-        <v>45425</v>
+        <v>45594</v>
       </c>
       <c r="E87" s="2" t="n">
-        <v>45474</v>
+        <v>45594</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
@@ -3358,7 +3358,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Tonto/ dates not needed TBD</t>
+          <t xml:space="preserve">FOR445 related field trip destination wilderness either in Sedona, Sycamore canyon, or around Flagstaff </t>
         </is>
       </c>
       <c r="H87" t="inlineStr"/>
@@ -3372,7 +3372,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>keven</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3381,10 +3381,10 @@
         </is>
       </c>
       <c r="D88" s="2" t="n">
-        <v>45629</v>
+        <v>45568</v>
       </c>
       <c r="E88" s="2" t="n">
-        <v>45648</v>
+        <v>45572</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
@@ -3393,14 +3393,10 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t xml:space="preserve">I will be traveling down to Casa Grande National Monument to join another NAU field crew and finish fieldwork on my research trip. This vehicle will transport one to two people at a time. The first destination is Casa Grande, followed by Tonto National Monument. </t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>Keven Griffen</t>
-        </is>
-      </c>
+          <t>sierra ancha</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr"/>
       <c r="I88" t="n">
         <v>95</v>
       </c>
@@ -3411,7 +3407,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Emory Ellis</t>
+          <t>Anita</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3420,10 +3416,10 @@
         </is>
       </c>
       <c r="D89" s="2" t="n">
-        <v>45610</v>
+        <v>45401</v>
       </c>
       <c r="E89" s="2" t="n">
-        <v>45614</v>
+        <v>45410</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
@@ -3442,7 +3438,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Bowker</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3451,21 +3447,17 @@
         </is>
       </c>
       <c r="D90" s="2" t="n">
-        <v>45605</v>
+        <v>45421</v>
       </c>
       <c r="E90" s="2" t="n">
-        <v>45605</v>
+        <v>45421</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
           <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Pick up materials from home depot </t>
-        </is>
-      </c>
+      <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr"/>
       <c r="I90" t="n">
         <v>93</v>
@@ -3477,7 +3469,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Anita</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3486,17 +3478,21 @@
         </is>
       </c>
       <c r="D91" s="2" t="n">
-        <v>45595</v>
+        <v>45425</v>
       </c>
       <c r="E91" s="2" t="n">
-        <v>45599</v>
+        <v>45534</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
           <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
-      <c r="G91" t="inlineStr"/>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>northern AZ, southern Utah, Lincoln, available most weekends/TBD</t>
+        </is>
+      </c>
       <c r="H91" t="inlineStr"/>
       <c r="I91" t="n">
         <v>92</v>
@@ -3508,7 +3504,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Lauren Orme</t>
+          <t>Derek Uhey</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3517,10 +3513,10 @@
         </is>
       </c>
       <c r="D92" s="2" t="n">
-        <v>45592</v>
+        <v>45561</v>
       </c>
       <c r="E92" s="2" t="n">
-        <v>45594</v>
+        <v>45561</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
@@ -3539,7 +3535,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Derek Uhey</t>
+          <t>Anita</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3548,10 +3544,10 @@
         </is>
       </c>
       <c r="D93" s="2" t="n">
-        <v>45561</v>
+        <v>45595</v>
       </c>
       <c r="E93" s="2" t="n">
-        <v>45561</v>
+        <v>45599</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
@@ -3570,7 +3566,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>Bowker</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3579,10 +3575,10 @@
         </is>
       </c>
       <c r="D94" s="2" t="n">
-        <v>45425</v>
+        <v>45605</v>
       </c>
       <c r="E94" s="2" t="n">
-        <v>45534</v>
+        <v>45605</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
@@ -3591,7 +3587,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>northern AZ, southern Utah, Lincoln, available most weekends/TBD</t>
+          <t xml:space="preserve">Pick up materials from home depot </t>
         </is>
       </c>
       <c r="H94" t="inlineStr"/>
@@ -3605,7 +3601,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>Emory Ellis</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3614,10 +3610,10 @@
         </is>
       </c>
       <c r="D95" s="2" t="n">
-        <v>45421</v>
+        <v>45610</v>
       </c>
       <c r="E95" s="2" t="n">
-        <v>45421</v>
+        <v>45614</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
@@ -3636,7 +3632,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Anita</t>
+          <t>keven</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3645,18 +3641,26 @@
         </is>
       </c>
       <c r="D96" s="2" t="n">
-        <v>45401</v>
+        <v>45629</v>
       </c>
       <c r="E96" s="2" t="n">
-        <v>45410</v>
+        <v>45648</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
           <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
-      <c r="G96" t="inlineStr"/>
-      <c r="H96" t="inlineStr"/>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I will be traveling down to Casa Grande National Monument to join another NAU field crew and finish fieldwork on my research trip. This vehicle will transport one to two people at a time. The first destination is Casa Grande, followed by Tonto National Monument. </t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Keven Griffen</t>
+        </is>
+      </c>
       <c r="I96" t="n">
         <v>86</v>
       </c>
@@ -3667,7 +3671,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>Lauren Orme</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3676,21 +3680,17 @@
         </is>
       </c>
       <c r="D97" s="2" t="n">
-        <v>45568</v>
+        <v>45592</v>
       </c>
       <c r="E97" s="2" t="n">
-        <v>45572</v>
+        <v>45594</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
           <t>466 - 2007 Ford Expedition, Silver (7 Seats)</t>
         </is>
       </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>sierra ancha</t>
-        </is>
-      </c>
+      <c r="G97" t="inlineStr"/>
       <c r="H97" t="inlineStr"/>
       <c r="I97" t="n">
         <v>90</v>
@@ -3702,7 +3702,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Kimberly Walker</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3711,21 +3711,17 @@
         </is>
       </c>
       <c r="D98" s="2" t="n">
-        <v>45496</v>
+        <v>45440</v>
       </c>
       <c r="E98" s="2" t="n">
-        <v>45506</v>
+        <v>45440</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
           <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
         </is>
       </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>southern AZ/NM</t>
-        </is>
-      </c>
+      <c r="G98" t="inlineStr"/>
       <c r="H98" t="inlineStr"/>
       <c r="I98" t="n">
         <v>103</v>
@@ -3737,7 +3733,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>Bowker</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3746,21 +3742,17 @@
         </is>
       </c>
       <c r="D99" s="2" t="n">
-        <v>45523</v>
+        <v>45401</v>
       </c>
       <c r="E99" s="2" t="n">
-        <v>45524</v>
+        <v>45402</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
           <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
         </is>
       </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 	Research day trip for data collection on Tonto NF. </t>
-        </is>
-      </c>
+      <c r="G99" t="inlineStr"/>
       <c r="H99" t="inlineStr"/>
       <c r="I99" t="n">
         <v>106</v>
@@ -3772,7 +3764,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>Michael Sloan</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3781,10 +3773,10 @@
         </is>
       </c>
       <c r="D100" s="2" t="n">
-        <v>45516</v>
+        <v>45408</v>
       </c>
       <c r="E100" s="2" t="n">
-        <v>45521</v>
+        <v>45412</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
@@ -3803,7 +3795,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>Salli Dymond</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3812,17 +3804,21 @@
         </is>
       </c>
       <c r="D101" s="2" t="n">
-        <v>45509</v>
+        <v>45431</v>
       </c>
       <c r="E101" s="2" t="n">
-        <v>45513</v>
+        <v>45436</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
           <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
         </is>
       </c>
-      <c r="G101" t="inlineStr"/>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sierra Ancha, </t>
+        </is>
+      </c>
       <c r="H101" t="inlineStr"/>
       <c r="I101" t="n">
         <v>104</v>
@@ -3834,7 +3830,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>CF</t>
+          <t>Waring</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3843,10 +3839,10 @@
         </is>
       </c>
       <c r="D102" s="2" t="n">
-        <v>45488</v>
+        <v>45441</v>
       </c>
       <c r="E102" s="2" t="n">
-        <v>45491</v>
+        <v>45442</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
@@ -3854,11 +3850,7 @@
         </is>
       </c>
       <c r="G102" t="inlineStr"/>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t>Shay Levine</t>
-        </is>
-      </c>
+      <c r="H102" t="inlineStr"/>
       <c r="I102" t="n">
         <v>102</v>
       </c>
@@ -3869,7 +3861,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>David Auty</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3878,10 +3870,10 @@
         </is>
       </c>
       <c r="D103" s="2" t="n">
-        <v>45527</v>
+        <v>45478</v>
       </c>
       <c r="E103" s="2" t="n">
-        <v>45527</v>
+        <v>45487</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -3890,7 +3882,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 	Field visit to Pump House Wash for Ironwood Forestry field demo. </t>
+          <t>southern AZ/NM</t>
         </is>
       </c>
       <c r="H103" t="inlineStr"/>
@@ -3904,7 +3896,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Waring</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3913,10 +3905,10 @@
         </is>
       </c>
       <c r="D104" s="2" t="n">
-        <v>45441</v>
+        <v>45488</v>
       </c>
       <c r="E104" s="2" t="n">
-        <v>45442</v>
+        <v>45491</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
@@ -3924,7 +3916,11 @@
         </is>
       </c>
       <c r="G104" t="inlineStr"/>
-      <c r="H104" t="inlineStr"/>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Shay Levine</t>
+        </is>
+      </c>
       <c r="I104" t="n">
         <v>100</v>
       </c>
@@ -3935,7 +3931,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Kimberly Walker</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3944,10 +3940,10 @@
         </is>
       </c>
       <c r="D105" s="2" t="n">
-        <v>45440</v>
+        <v>45509</v>
       </c>
       <c r="E105" s="2" t="n">
-        <v>45440</v>
+        <v>45513</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -3966,7 +3962,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Salli Dymond</t>
+          <t>CF</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3975,21 +3971,17 @@
         </is>
       </c>
       <c r="D106" s="2" t="n">
-        <v>45431</v>
+        <v>45516</v>
       </c>
       <c r="E106" s="2" t="n">
-        <v>45436</v>
+        <v>45521</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
           <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
         </is>
       </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Sierra Ancha, </t>
-        </is>
-      </c>
+      <c r="G106" t="inlineStr"/>
       <c r="H106" t="inlineStr"/>
       <c r="I106" t="n">
         <v>98</v>
@@ -4001,7 +3993,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Michael Sloan</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -4010,17 +4002,21 @@
         </is>
       </c>
       <c r="D107" s="2" t="n">
-        <v>45408</v>
+        <v>45523</v>
       </c>
       <c r="E107" s="2" t="n">
-        <v>45412</v>
+        <v>45524</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
           <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
         </is>
       </c>
-      <c r="G107" t="inlineStr"/>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 	Research day trip for data collection on Tonto NF. </t>
+        </is>
+      </c>
       <c r="H107" t="inlineStr"/>
       <c r="I107" t="n">
         <v>97</v>
@@ -4032,7 +4028,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Bowker</t>
+          <t xml:space="preserve">Pete Fule </t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -4041,17 +4037,21 @@
         </is>
       </c>
       <c r="D108" s="2" t="n">
-        <v>45401</v>
+        <v>45496</v>
       </c>
       <c r="E108" s="2" t="n">
-        <v>45402</v>
+        <v>45506</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
           <t>467 - 2011 Chevy Silverado, Pearl (5 Seats)</t>
         </is>
       </c>
-      <c r="G108" t="inlineStr"/>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>southern AZ/NM</t>
+        </is>
+      </c>
       <c r="H108" t="inlineStr"/>
       <c r="I108" t="n">
         <v>96</v>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pete Fule </t>
+          <t>David Auty</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -4072,10 +4072,10 @@
         </is>
       </c>
       <c r="D109" s="2" t="n">
-        <v>45478</v>
+        <v>45527</v>
       </c>
       <c r="E109" s="2" t="n">
-        <v>45487</v>
+        <v>45527</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>southern AZ/NM</t>
+          <t xml:space="preserve"> 	Field visit to Pump House Wash for Ironwood Forestry field demo. </t>
         </is>
       </c>
       <c r="H109" t="inlineStr"/>

</xml_diff>